<commit_message>
tarefa 0050 pessoas completada
</commit_message>
<xml_diff>
--- a/agenda.xlsx
+++ b/agenda.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meira\Projetos\Padaria\padaria-doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renan\Projetos\Padaria\padaria-doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCD287A-C79B-4788-8501-0CEB294FCD01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB207914-019A-46EE-9179-8B2AF63087E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{69933DCC-ED01-7C44-8F70-AA2271B99551}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{69933DCC-ED01-7C44-8F70-AA2271B99551}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -695,19 +695,19 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
-    <col min="2" max="4" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="16.8984375" customWidth="1"/>
+    <col min="2" max="4" width="14.59765625" customWidth="1"/>
     <col min="5" max="5" width="16.5" customWidth="1"/>
     <col min="6" max="6" width="32.5" customWidth="1"/>
-    <col min="7" max="7" width="45.125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="45.09765625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -730,7 +730,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -739,7 +739,7 @@
       </c>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -762,7 +762,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -785,7 +785,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -805,7 +805,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -818,6 +818,9 @@
       <c r="D6" s="2">
         <v>45154</v>
       </c>
+      <c r="E6" s="2">
+        <v>45152</v>
+      </c>
       <c r="F6" t="s">
         <v>15</v>
       </c>
@@ -825,7 +828,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -845,7 +848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -865,7 +868,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -885,7 +888,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -905,7 +908,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -925,7 +928,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -945,7 +948,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -965,7 +968,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -985,7 +988,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1005,7 +1008,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1025,7 +1028,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1045,7 +1048,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1065,7 +1068,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -1074,7 +1077,7 @@
       </c>
       <c r="G19" s="9"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1094,7 +1097,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1114,7 +1117,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1134,7 +1137,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1154,7 +1157,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1174,7 +1177,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1194,7 +1197,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1214,7 +1217,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1234,7 +1237,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1254,7 +1257,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1274,7 +1277,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1294,7 +1297,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1314,7 +1317,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1334,7 +1337,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -1354,7 +1357,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1374,7 +1377,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -1391,7 +1394,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -1411,7 +1414,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -1431,7 +1434,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -1451,7 +1454,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -1471,7 +1474,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -1491,7 +1494,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -1511,7 +1514,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -1531,7 +1534,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -1551,7 +1554,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -1571,7 +1574,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -1591,7 +1594,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
tarefa 0050 pessoas concluida, AJ
</commit_message>
<xml_diff>
--- a/agenda.xlsx
+++ b/agenda.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renan\Projetos\Padaria\padaria-doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB207914-019A-46EE-9179-8B2AF63087E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA13BBEF-466F-4441-8750-586525FE2248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{69933DCC-ED01-7C44-8F70-AA2271B99551}"/>
   </bookViews>
@@ -695,7 +695,7 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -798,6 +798,9 @@
       <c r="D5" s="2">
         <v>45154</v>
       </c>
+      <c r="E5" s="2">
+        <v>45152</v>
+      </c>
       <c r="F5" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Data conclusao tarefa Pagar adicionada
</commit_message>
<xml_diff>
--- a/agenda.xlsx
+++ b/agenda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renan\Projetos\Padaria\padaria-doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA13BBEF-466F-4441-8750-586525FE2248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DCB493-C459-4EDA-8884-098C610796F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{69933DCC-ED01-7C44-8F70-AA2271B99551}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{69933DCC-ED01-7C44-8F70-AA2271B99551}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -694,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80441D6D-8D39-D14B-AE2A-18541D22F157}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -884,6 +884,9 @@
       <c r="D9" s="2">
         <v>45154</v>
       </c>
+      <c r="E9" s="2">
+        <v>45153</v>
+      </c>
       <c r="F9" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Adicionado data de conclusao da tarefa 0200
</commit_message>
<xml_diff>
--- a/agenda.xlsx
+++ b/agenda.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meira\Projetos\Padaria\padaria-doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E15DFCC-049C-4739-81F7-C5975E76B403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41433C5-9362-4C6E-9D8B-189A3F8CDEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{69933DCC-ED01-7C44-8F70-AA2271B99551}"/>
   </bookViews>
@@ -695,7 +695,7 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -910,6 +910,9 @@
       <c r="D10" s="2">
         <v>45154</v>
       </c>
+      <c r="E10" s="2">
+        <v>45153</v>
+      </c>
       <c r="F10" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Atualizado conclusao de tarefa AJ
</commit_message>
<xml_diff>
--- a/agenda.xlsx
+++ b/agenda.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meira\Projetos\Padaria\padaria-doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41433C5-9362-4C6E-9D8B-189A3F8CDEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73788D94-D9DE-465C-872B-35B68011CB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{69933DCC-ED01-7C44-8F70-AA2271B99551}"/>
   </bookViews>
@@ -694,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80441D6D-8D39-D14B-AE2A-18541D22F157}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -867,6 +867,9 @@
       <c r="D8" s="2">
         <v>45154</v>
       </c>
+      <c r="E8" s="2">
+        <v>45153</v>
+      </c>
       <c r="F8" t="s">
         <v>17</v>
       </c>
@@ -932,6 +935,9 @@
       </c>
       <c r="D11" s="2">
         <v>45154</v>
+      </c>
+      <c r="E11" s="2">
+        <v>45153</v>
       </c>
       <c r="F11" t="s">
         <v>22</v>

</xml_diff>